<commit_message>
Pushing this broken ass thing to main
</commit_message>
<xml_diff>
--- a/app/data/Summary_Data.xlsx
+++ b/app/data/Summary_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://meridianenergy-my.sharepoint.com/personal/russell_chubb_meridianenergy_co_nz/Documents/Documents/Programming/Personal/Golf_Stats_App/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://meridianenergy-my.sharepoint.com/personal/russell_chubb_meridianenergy_co_nz/Documents/Documents/Programming/Personal/Golf_Stats_App/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="11_F25DC773A252ABDACC104822F95A42B45BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4D64659-201B-4D5A-9DB2-15B0F29ABD7E}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="11_F25DC773A252ABDACC104822F95A42B45BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20323630-8DEE-44A6-86C9-962C9474FBD4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29970" yWindow="1170" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>Is this my best score yet? - (Technically the back 9 of the 18 on 4/10/2025 was better +13)</t>
+  </si>
+  <si>
+    <t>Masterton Golf Course</t>
+  </si>
+  <si>
+    <t>Practice</t>
+  </si>
+  <si>
+    <t>Only played 8, adjusted score and par for course to account</t>
   </si>
 </sst>
 </file>
@@ -439,16 +448,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="A1:I2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="81.7109375" bestFit="1" customWidth="1"/>
@@ -485,10 +494,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45948</v>
+        <v>45950</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -497,25 +506,26 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F2">
+        <f>SUM(6+6+5+8+7+5+6+6)</f>
         <v>49</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H2">
         <f>SUM(F2-G2)</f>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45942</v>
+        <v>45948</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -530,19 +540,22 @@
         <v>19</v>
       </c>
       <c r="F3">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G3">
         <v>30</v>
       </c>
       <c r="H3">
         <f>SUM(F3-G3)</f>
-        <v>29</v>
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45934</v>
+        <v>45942</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -551,28 +564,25 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="G4">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="H4">
         <f>SUM(F4-G4)</f>
-        <v>50</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45913</v>
+        <v>45934</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -581,25 +591,28 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
       <c r="F5">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="H5">
         <f>SUM(F5-G5)</f>
-        <v>28</v>
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>45912</v>
+        <v>45913</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -608,25 +621,25 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
       <c r="F6">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="G6">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H6">
         <f>SUM(F6-G6)</f>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>45910</v>
+        <v>45912</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -635,25 +648,25 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
       </c>
       <c r="F7">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H7">
         <f>SUM(F7-G7)</f>
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>45864</v>
+        <v>45910</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -662,23 +675,20 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
       </c>
       <c r="F8">
-        <v>140</v>
+        <v>57</v>
       </c>
       <c r="G8">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="H8">
         <f>SUM(F8-G8)</f>
-        <v>68</v>
-      </c>
-      <c r="I8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -689,7 +699,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -698,41 +708,44 @@
         <v>19</v>
       </c>
       <c r="F9">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="G9">
         <v>72</v>
       </c>
       <c r="H9">
         <f>SUM(F9-G9)</f>
-        <v>48</v>
+        <v>68</v>
+      </c>
+      <c r="I9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>45857</v>
+        <v>45864</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
         <v>19</v>
       </c>
       <c r="F10">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="G10">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="H10">
         <f>SUM(F10-G10)</f>
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -743,7 +756,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -752,28 +765,25 @@
         <v>19</v>
       </c>
       <c r="F11">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G11">
         <v>30</v>
       </c>
       <c r="H11">
         <f>SUM(F11-G11)</f>
-        <v>13</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>45836</v>
+        <v>45857</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -782,14 +792,17 @@
         <v>19</v>
       </c>
       <c r="F12">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G12">
         <v>30</v>
       </c>
       <c r="H12">
         <f>SUM(F12-G12)</f>
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -800,7 +813,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -821,34 +834,61 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>45787</v>
+        <v>45836</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="G14">
         <v>30</v>
       </c>
       <c r="H14">
         <f>SUM(F14-G14)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45787</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>38</v>
+      </c>
+      <c r="G15">
+        <v>30</v>
+      </c>
+      <c r="H15">
+        <f>SUM(F15-G15)</f>
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I8" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I14">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I15">
       <sortCondition descending="1" ref="A1:A8"/>
     </sortState>
   </autoFilter>

</xml_diff>